<commit_message>
corrected the csv folder
</commit_message>
<xml_diff>
--- a/TestDataAndResults/SophieAutomation.xlsx
+++ b/TestDataAndResults/SophieAutomation.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{6756726C-8FCC-4B16-BD4D-355CD0B4A303}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39794AA2-C33D-4EE3-89AF-0205132A290E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="DriverSheet" r:id="rId1" sheetId="1"/>
-    <sheet name="CSVChkPostDefineBrain" r:id="rId2" sheetId="4"/>
-    <sheet name="BatchDecisionOutputValidations" r:id="rId3" sheetId="5"/>
-    <sheet name="Keywords" r:id="rId4" sheetId="3"/>
+    <sheet name="DriverSheet" sheetId="1" r:id="rId1"/>
+    <sheet name="CSVChkPostDefineBrain" sheetId="4" r:id="rId2"/>
+    <sheet name="BatchDecisionOutputValidations" sheetId="5" r:id="rId3"/>
+    <sheet name="Keywords" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="195">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -607,9 +607,6 @@
     <t>Choose obcc template</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
     <t>Module</t>
   </si>
   <si>
@@ -617,16 +614,12 @@
   </si>
   <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -780,60 +773,60 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="4" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="25">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="4" numFmtId="0" quotePrefix="1" xfId="1"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="3" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="3" fontId="3" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="3" fontId="3" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="3" fontId="3" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="3" fontId="3" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -850,10 +843,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -888,7 +881,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -923,7 +916,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1017,21 +1010,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1048,7 +1041,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1100,15 +1093,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
@@ -1116,15 +1109,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="23.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="70.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="19.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="24.42578125" collapsed="true"/>
-    <col min="6" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="70.7109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.42578125" style="3" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" ht="14.25" r="1" s="6" spans="1:5">
+    <row r="1" spans="1:5" s="6" customFormat="1" ht="14.25">
       <c r="A1" s="17" t="s">
         <v>35</v>
       </c>
@@ -1133,7 +1126,7 @@
       <c r="D1" s="17"/>
       <c r="E1" s="17"/>
     </row>
-    <row customFormat="1" ht="14.25" r="2" s="6" spans="1:5">
+    <row r="2" spans="1:5" s="6" customFormat="1" ht="14.25">
       <c r="A2" s="18" t="s">
         <v>187</v>
       </c>
@@ -1142,19 +1135,19 @@
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
     </row>
-    <row customFormat="1" ht="14.25" r="3" s="6" spans="1:5">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="14.25">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row customFormat="1" ht="14.25" r="4" s="2" spans="1:5">
+    <row r="4" spans="1:5" s="2" customFormat="1" ht="14.25">
       <c r="A4" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>1</v>
@@ -1171,7 +1164,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>58</v>
@@ -1186,13 +1179,13 @@
         <v>138</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>139</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E6" s="4"/>
     </row>
@@ -1201,27 +1194,27 @@
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EA4E71-0B53-4881-A15A-C454293CD34C}">
-  <dimension ref="A1:H80"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EA4E71-0B53-4881-A15A-C454293CD34C}">
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:G31"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="G67" sqref="G67:G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="39.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="32.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="7.86328125" collapsed="true"/>
+    <col min="1" max="1" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="39" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1293,9 +1286,7 @@
         <v>69</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="4" t="s">
-        <v>196</v>
-      </c>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="4" t="s">
@@ -1855,9 +1846,7 @@
         <v>70</v>
       </c>
       <c r="F33" s="4"/>
-      <c r="G33" s="4" t="s">
-        <v>192</v>
-      </c>
+      <c r="G33" s="4"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="4" t="s">
@@ -2786,26 +2775,26 @@
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A3:G3"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38793A77-4CB9-44FE-853A-5596922718C4}">
-  <dimension ref="A1:H8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38793A77-4CB9-44FE-853A-5596922718C4}">
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2867,9 +2856,6 @@
       <c r="D5" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E5" t="s">
-        <v>192</v>
-      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="9" t="s">
@@ -2884,9 +2870,6 @@
       <c r="D6" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E6" t="s">
-        <v>192</v>
-      </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="9" t="s">
@@ -2901,9 +2884,6 @@
       <c r="D7" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E7" t="s">
-        <v>192</v>
-      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="9" t="s">
@@ -2917,9 +2897,6 @@
       </c>
       <c r="D8" s="9" t="s">
         <v>122</v>
-      </c>
-      <c r="E8" t="s">
-        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -2928,13 +2905,13 @@
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A3:G3"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0813C85-E9CB-4B87-91F1-B57B26429AF3}">
-  <dimension ref="A1:E15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0813C85-E9CB-4B87-91F1-B57B26429AF3}">
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
@@ -2942,12 +2919,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="1" max="1" width="22" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:4">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2981,7 +2958,7 @@
         <v>15</v>
       </c>
       <c r="D3" t="str">
-        <f ref="D3:D15" si="0" t="shared">_xlfn.CONCAT(A3,B3)</f>
+        <f t="shared" ref="D3:D15" si="0">_xlfn.CONCAT(A3,B3)</f>
         <v>LinkClick</v>
       </c>
     </row>
@@ -2993,7 +2970,7 @@
         <v>15</v>
       </c>
       <c r="D4" t="str">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>ButtonClick</v>
       </c>
     </row>
@@ -3005,7 +2982,7 @@
         <v>18</v>
       </c>
       <c r="D5" t="str">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>DropdownSelect</v>
       </c>
     </row>
@@ -3017,7 +2994,7 @@
         <v>20</v>
       </c>
       <c r="D6" t="str">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>Text/LabelRead</v>
       </c>
     </row>
@@ -3029,7 +3006,7 @@
         <v>18</v>
       </c>
       <c r="D7" t="str">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>RadioSelect</v>
       </c>
     </row>
@@ -3041,7 +3018,7 @@
         <v>23</v>
       </c>
       <c r="D8" t="str">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>CheckBoxCheck</v>
       </c>
     </row>
@@ -3053,7 +3030,7 @@
         <v>24</v>
       </c>
       <c r="D9" t="str">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>CheckBoxUncheck</v>
       </c>
     </row>
@@ -3065,7 +3042,7 @@
         <v>15</v>
       </c>
       <c r="D10" t="str">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>ImagebuttonClick</v>
       </c>
     </row>
@@ -3074,7 +3051,7 @@
         <v>26</v>
       </c>
       <c r="D11" t="str">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>Table</v>
       </c>
     </row>
@@ -3086,7 +3063,7 @@
         <v>28</v>
       </c>
       <c r="D12" t="str">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>BrowserOpen</v>
       </c>
     </row>
@@ -3098,7 +3075,7 @@
         <v>29</v>
       </c>
       <c r="D13" t="str">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>BrowserClose</v>
       </c>
     </row>
@@ -3110,7 +3087,7 @@
         <v>30</v>
       </c>
       <c r="D14" t="str">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>BrowserNavigate</v>
       </c>
     </row>
@@ -3122,11 +3099,11 @@
         <v>32</v>
       </c>
       <c r="D15" t="str">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
         <v>ElementPropertyCheck</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>